<commit_message>
changes in test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/unit.xlsx
+++ b/src/main/resources/unit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jiofabric\Selenium-java\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B14AE3-D3F5-499D-BE08-4A817FB6BDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB9A13C-309D-4C36-92AF-AE200A71D697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="2415" windowWidth="18000" windowHeight="9360" xr2:uid="{04E55122-9D7C-482F-A624-2D17462FB4FA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>CyberSecurity</t>
   </si>
   <si>
-    <t>asd3</t>
-  </si>
-  <si>
     <t>asd4</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>asd11</t>
   </si>
   <si>
-    <t>uiop3</t>
-  </si>
-  <si>
     <t>uiop4</t>
   </si>
   <si>
@@ -148,25 +142,25 @@
     <t>Retail</t>
   </si>
   <si>
-    <t>asd222</t>
-  </si>
-  <si>
-    <t>uiop22</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>drrr</t>
-  </si>
-  <si>
-    <t>fserrr</t>
-  </si>
-  <si>
     <t>u1,U1, d1</t>
   </si>
   <si>
     <t>dred</t>
+  </si>
+  <si>
+    <t>srusi</t>
+  </si>
+  <si>
+    <t>ftgi</t>
+  </si>
+  <si>
+    <t>sdit</t>
+  </si>
+  <si>
+    <t>udyth</t>
   </si>
 </sst>
 </file>
@@ -521,7 +515,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,16 +551,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -576,12 +570,6 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
@@ -589,18 +577,18 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -609,7 +597,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -617,10 +605,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -629,7 +617,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -637,10 +625,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -649,7 +637,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -657,10 +645,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -669,7 +657,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -677,10 +665,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -689,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,10 +685,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -709,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -717,10 +705,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -729,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -737,10 +725,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -749,7 +737,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -757,10 +745,10 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -769,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>